<commit_message>
Commit : Created final conditions, so each row's end has the OK,Hiba,Nem talált message
</commit_message>
<xml_diff>
--- a/AbesseHomeWork/BeerIbuExcel.xlsx
+++ b/AbesseHomeWork/BeerIbuExcel.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AbesseHomeWork\AbesseHomeWork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9560BC8A-AC5F-4A6C-9718-72B351EE917A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Munka1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +25,181 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+  <si>
+    <t>Buzz</t>
+  </si>
+  <si>
+    <t>60 IBU</t>
+  </si>
+  <si>
+    <t>20 IBU</t>
+  </si>
+  <si>
+    <t>Hiba</t>
+  </si>
+  <si>
+    <t>Trashy Blonde</t>
+  </si>
+  <si>
+    <t>41.5 IBU</t>
+  </si>
+  <si>
+    <t>40 IBU</t>
+  </si>
+  <si>
+    <t>Berliner Weisse With Yuzu - B-Sides</t>
+  </si>
+  <si>
+    <t>8 IBU</t>
+  </si>
+  <si>
+    <t>Beer not existing in Source_2</t>
+  </si>
+  <si>
+    <t>Nem található</t>
+  </si>
+  <si>
+    <t>Pilsen Lager</t>
+  </si>
+  <si>
+    <t>55 IBU</t>
+  </si>
+  <si>
+    <t>22 IBU</t>
+  </si>
+  <si>
+    <t>Avery Brown Dredge</t>
+  </si>
+  <si>
+    <t>59 IBU</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Electric India</t>
+  </si>
+  <si>
+    <t>38 IBU</t>
+  </si>
+  <si>
+    <t>AB:12</t>
+  </si>
+  <si>
+    <t>35 IBU</t>
+  </si>
+  <si>
+    <t>16 IBU</t>
+  </si>
+  <si>
+    <t>Fake Lager</t>
+  </si>
+  <si>
+    <t>37 IBU</t>
+  </si>
+  <si>
+    <t>AB:07</t>
+  </si>
+  <si>
+    <t>30 IBU</t>
+  </si>
+  <si>
+    <t>N/A IBU</t>
+  </si>
+  <si>
+    <t>Bramling X</t>
+  </si>
+  <si>
+    <t>75 IBU</t>
+  </si>
+  <si>
+    <t>Misspent Youth</t>
+  </si>
+  <si>
+    <t>Arcade Nation</t>
+  </si>
+  <si>
+    <t>50 IBU</t>
+  </si>
+  <si>
+    <t>Movember</t>
+  </si>
+  <si>
+    <t>Alpha Dog</t>
+  </si>
+  <si>
+    <t>42 IBU</t>
+  </si>
+  <si>
+    <t>126 IBU</t>
+  </si>
+  <si>
+    <t>Mixtape 8</t>
+  </si>
+  <si>
+    <t>Libertine Porter</t>
+  </si>
+  <si>
+    <t>45 IBU</t>
+  </si>
+  <si>
+    <t>AB:06</t>
+  </si>
+  <si>
+    <t>150 IBU</t>
+  </si>
+  <si>
+    <t>Russian Doll – India Pale Ale</t>
+  </si>
+  <si>
+    <t>70 IBU</t>
+  </si>
+  <si>
+    <t>Hello My Name Is Mette-Marit</t>
+  </si>
+  <si>
+    <t>Rabiator</t>
+  </si>
+  <si>
+    <t>26 IBU</t>
+  </si>
+  <si>
+    <t>Vice Bier</t>
+  </si>
+  <si>
+    <t>25 IBU</t>
+  </si>
+  <si>
+    <t>19 IBU</t>
+  </si>
+  <si>
+    <t>Devine Rebel (w/ Mikkeller)</t>
+  </si>
+  <si>
+    <t>100 IBU</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>65 IBU</t>
+  </si>
+  <si>
+    <t>The End Of History</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IBU</t>
+  </si>
+  <si>
+    <t>Bad Pixie</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,10 +510,379 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6801EB-B64B-4C1C-A20C-CEB25EFC335F}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="75.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Commit : Updated the while loop, so it's going to work with any jsonArray length
</commit_message>
<xml_diff>
--- a/AbesseHomeWork/BeerIbuExcel.xlsx
+++ b/AbesseHomeWork/BeerIbuExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AbesseHomeWork\AbesseHomeWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9560BC8A-AC5F-4A6C-9718-72B351EE917A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3417C3-A83D-4DD1-8D33-915E169BB080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,12 +514,14 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="75.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>